<commit_message>
Update Front-End for Products page
</commit_message>
<xml_diff>
--- a/Document/SWP391-AppDevProject_Backlog Template.xlsx
+++ b/Document/SWP391-AppDevProject_Backlog Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25718"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiennt/FeStore/MyDrive/MyWorks/FU/SWP391-Project/Guides_Student/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27C40A0F-0B0D-4D6F-96F7-12B948D5DFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C171BCC2-68F6-46B3-80A8-AAC0AE72B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14880" xr2:uid="{DF743DC6-3E10-FC40-A74C-7ADFA9B03788}"/>
   </bookViews>

</xml_diff>